<commit_message>
Navision issue fixed and Running upto submit
</commit_message>
<xml_diff>
--- a/MDM_POC/input/data/Global_Material_Data.xlsx
+++ b/MDM_POC/input/data/Global_Material_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Downloads\MDM_POC_Upgrade\MDM_POC_Upgrade\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git\MDM_TEST\MDM_POC\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E305710-7E35-438C-8511-81030C52140C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{731C1130-06F4-4485-A83F-9CE7196BFDCC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" xr2:uid="{92753D1E-95E7-49CB-AD96-B588CC3DB29F}"/>
   </bookViews>
@@ -258,9 +258,6 @@
     <t>NL</t>
   </si>
   <si>
-    <t>Lens Niet Verlicht 82mm MAES 2017</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
@@ -330,7 +327,10 @@
     <t>.</t>
   </si>
   <si>
-    <t>Lens Non Illuminated 82mm MAES 2018</t>
+    <t>Lens Non Illuminated 82mm MAES 2016</t>
+  </si>
+  <si>
+    <t>Lens Niet Verlicht 82mm MAES 2016</t>
   </si>
 </sst>
 </file>
@@ -817,14 +817,14 @@
   <dimension ref="A1:FC9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -992,7 +992,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>4</v>
@@ -1445,50 +1445,50 @@
         <v>74</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>75</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>76</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>86</v>
-      </c>
       <c r="Q2" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -1598,77 +1598,77 @@
       <c r="DS2" s="6"/>
       <c r="DT2" s="6"/>
       <c r="DU2" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="DV2" s="6"/>
       <c r="DW2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="DX2" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="DX2" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="DY2" s="6"/>
       <c r="DZ2" s="6"/>
       <c r="EA2" s="6"/>
       <c r="EB2" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="EC2" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="ED2" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="EE2" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="EF2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="EG2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="EH2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="EI2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="EJ2" s="6"/>
       <c r="EK2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="EL2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="EL2" s="6" t="s">
+      <c r="EM2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="EN2" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="EM2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="EN2" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="EO2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="EP2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="EQ2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="ER2" s="6"/>
       <c r="ES2" s="6"/>
       <c r="ET2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="EU2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="EU2" s="6" t="s">
+      <c r="EV2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="EW2" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="EV2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="EW2" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="EX2" s="6"/>
       <c r="EY2" s="6"/>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="9" spans="1:159" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>